<commit_message>
schema spacing & contract excel changes
</commit_message>
<xml_diff>
--- a/backend/data/contracts/all_info.xlsx
+++ b/backend/data/contracts/all_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\web_application\backend\data\contracts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\MY_PROJECTS\web_application\backend\data\contracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFCDF18-8B10-4019-9109-BFC86850AEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EC1683-C0BC-4782-BA91-E7A5D8281BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5955" yWindow="-60" windowWidth="12000" windowHeight="17400" firstSheet="3" activeTab="4" xr2:uid="{4AAAB276-E881-4B9F-B447-DB4F3993933A}"/>
+    <workbookView minimized="1" xWindow="4590" yWindow="4395" windowWidth="14745" windowHeight="7815" activeTab="4" xr2:uid="{4AAAB276-E881-4B9F-B447-DB4F3993933A}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Stages" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>Preliminaries</t>
   </si>
@@ -190,37 +190,49 @@
     <t>Removing Trees</t>
   </si>
   <si>
-    <t>m2</t>
-  </si>
-  <si>
     <t>nr</t>
   </si>
   <si>
-    <t>Nr</t>
-  </si>
-  <si>
     <t>Column Footing  4' 0" x 4' 0"x 3' 0"</t>
   </si>
   <si>
     <t xml:space="preserve">Column pit Excavation </t>
   </si>
   <si>
-    <t>m3</t>
-  </si>
-  <si>
     <t>Wall Tranches</t>
   </si>
   <si>
     <t>Water Disposal</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Erathwork supports</t>
-  </si>
-  <si>
     <t>Backfilling</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>cube</t>
+  </si>
+  <si>
+    <t>Screed concrete</t>
+  </si>
+  <si>
+    <t>Form work</t>
+  </si>
+  <si>
+    <t>Reinforcement</t>
+  </si>
+  <si>
+    <t>ft2</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>slab concrete</t>
+  </si>
+  <si>
+    <t>bag</t>
   </si>
 </sst>
 </file>
@@ -230,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +254,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -266,8 +286,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{382620F7-0C49-453B-9B48-E6E386CE9E1E}"/>
@@ -902,10 +923,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478CDEF1-FC80-40D9-9538-CC89BE1B9C14}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +936,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -935,7 +956,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -945,7 +966,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -954,7 +975,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -962,143 +983,186 @@
         <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>63</v>
       </c>
-      <c r="B17" t="s">
-        <v>58</v>
+      <c r="B21" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
+      <c r="A25" s="1"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
+      <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
+      <c r="A27" s="1"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
+      <c r="A28" s="1"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
+      <c r="A29" s="1"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>38</v>
-      </c>
+      <c r="A30" s="1"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>